<commit_message>
Make sure inventory UI matches with the real inventory
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterLocalization.xlsx
+++ b/Assets/Data/Excel/MasterLocalization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007C8571-77AF-4738-AB38-28B62EDFBD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC05484D-3368-42CC-904B-B662AEC0EA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -124,9 +124,6 @@
     <t>これはアイテム２</t>
   </si>
   <si>
-    <t>パズルブロッカだ。パズル用みたいです。</t>
-  </si>
-  <si>
     <t>扉のカギ</t>
   </si>
   <si>
@@ -137,6 +134,15 @@
   </si>
   <si>
     <t>Cという名前の本。</t>
+  </si>
+  <si>
+    <t>パズルBなもの</t>
+  </si>
+  <si>
+    <t>Aパズルブロッカだ。パズル用みたいです。</t>
+  </si>
+  <si>
+    <t>Bパズルブロッカだ。パズル用みたいです。</t>
   </si>
 </sst>
 </file>
@@ -551,7 +557,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,7 +640,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -704,7 +710,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +774,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -782,7 +788,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -796,7 +802,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -810,7 +816,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -824,7 +830,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -838,7 +844,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the dialogue response quest(still need testing) + localization for quest descriptions
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterLocalization.xlsx
+++ b/Assets/Data/Excel/MasterLocalization.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D47481-297B-4118-BD93-7EBC4D0E8495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F40CDC0-4234-4F1F-9930-F967928BDA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
   <sheets>
-    <sheet name="NameTextEntities" sheetId="1" r:id="rId1"/>
-    <sheet name="DescriptionTextEntities" sheetId="2" r:id="rId2"/>
+    <sheet name="NameEntities" sheetId="1" r:id="rId1"/>
+    <sheet name="DescriptionEntities" sheetId="2" r:id="rId2"/>
+    <sheet name="QuestNameEntities" sheetId="5" r:id="rId3"/>
+    <sheet name="QuestDescriptionEntities" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -164,13 +166,61 @@
   </si>
   <si>
     <t>ただのコイン</t>
+  </si>
+  <si>
+    <t>en01</t>
+  </si>
+  <si>
+    <t>en02</t>
+  </si>
+  <si>
+    <t>en03</t>
+  </si>
+  <si>
+    <t>jp01</t>
+  </si>
+  <si>
+    <t>jp02</t>
+  </si>
+  <si>
+    <t>jp03</t>
+  </si>
+  <si>
+    <t>Call my father?</t>
+  </si>
+  <si>
+    <t>Scavenge for coins.</t>
+  </si>
+  <si>
+    <t>Purchase Amulet from the vending machine</t>
+  </si>
+  <si>
+    <t>An unknown presence..</t>
+  </si>
+  <si>
+    <t>Economic hardship</t>
+  </si>
+  <si>
+    <t>未知の存在</t>
+  </si>
+  <si>
+    <t>びんぼう</t>
+  </si>
+  <si>
+    <t>パパを連絡</t>
+  </si>
+  <si>
+    <t>小銭を探せ</t>
+  </si>
+  <si>
+    <t>自動販売機でアミュレットを購入する</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +249,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +285,13 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -252,24 +314,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
@@ -587,7 +667,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,7 +815,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B1" sqref="B1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,4 +950,126 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA242C5-2C34-437D-BB92-AAC05F3C7C45}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>25000</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029577D5-7BE8-405C-850A-C637CD0444F1}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="7" width="4.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>25000</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Localized for quest display
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterLocalization.xlsx
+++ b/Assets/Data/Excel/MasterLocalization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F40CDC0-4234-4F1F-9930-F967928BDA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4442152D-4C91-40EE-8887-33D49839DCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
   <sheets>
     <sheet name="NameEntities" sheetId="1" r:id="rId1"/>
@@ -666,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA242C5-2C34-437D-BB92-AAC05F3C7C45}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Create a debug class to handle Debug log for debug/release
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterLocalization.xlsx
+++ b/Assets/Data/Excel/MasterLocalization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4442152D-4C91-40EE-8887-33D49839DCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A6DC31-FD8C-42BD-B329-A2E21C0FAE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
   <sheets>
     <sheet name="NameEntities" sheetId="1" r:id="rId1"/>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,11 +956,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA242C5-2C34-437D-BB92-AAC05F3C7C45}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -975,7 +978,7 @@
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>20000</v>
+        <v>20001</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>52</v>
@@ -1005,7 +1008,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1046,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>20000</v>
+        <v>20001</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>49</v>

</xml_diff>